<commit_message>
add Home explanation and expander in visualisation
</commit_message>
<xml_diff>
--- a/Doc/Emulsion_Recap.xlsx
+++ b/Doc/Emulsion_Recap.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Bureau\Moi\Efrei\Imbartabac\Programme\Assistanat_Project\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F78CCC8F-E3B9-4D94-AEF9-3FCC86C8420B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12680A-AAD5-4341-B1C8-1A220692DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
   </bookViews>
   <sheets>
     <sheet name="Récapitulatif" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="xcir0" hidden="1">-3.1415926536+(ROW(OFFSET(#REF!,0,0,500,1))-1)*0.0125915537</definedName>
     <definedName name="xdata1" hidden="1">-2782.6483723077+(ROW(OFFSET(#REF!,0,0,70,1))-1)*89.9736513266</definedName>
@@ -1256,62 +1253,62 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,28 +1325,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Modèle"/>
-      <sheetName val="Analyse Sensorielle"/>
-      <sheetName val="Mesures Instrumentales"/>
-      <sheetName val="Statistiques"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1652,10 +1627,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:AQ16"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1672,1966 +1647,1967 @@
     <col min="40" max="16384" width="12.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="93"/>
-      <c r="B1" s="92" t="s">
+    <row r="1" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="75"/>
+      <c r="B2" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="89" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="88"/>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="86" t="s">
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86"/>
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86"/>
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="87"/>
+      <c r="AJ2" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
-      <c r="AM1" s="85"/>
-      <c r="AN1" s="85"/>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="84"/>
+      <c r="AK2" s="89"/>
+      <c r="AL2" s="89"/>
+      <c r="AM2" s="89"/>
+      <c r="AN2" s="89"/>
+      <c r="AO2" s="89"/>
+      <c r="AP2" s="89"/>
+      <c r="AQ2" s="90"/>
     </row>
-    <row r="2" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="83"/>
-      <c r="B2" s="82" t="s">
+    <row r="3" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="74"/>
+      <c r="B3" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="81" t="s">
+      <c r="F3" s="78"/>
+      <c r="G3" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="82" t="s">
+      <c r="H3" s="77"/>
+      <c r="I3" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="80"/>
-      <c r="K2" s="82" t="s">
+      <c r="J3" s="78"/>
+      <c r="K3" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="79" t="s">
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="79" t="s">
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="76" t="s">
+      <c r="AB3" s="80"/>
+      <c r="AC3" s="80"/>
+      <c r="AD3" s="80"/>
+      <c r="AE3" s="80"/>
+      <c r="AF3" s="80"/>
+      <c r="AG3" s="80"/>
+      <c r="AH3" s="80"/>
+      <c r="AI3" s="81"/>
+      <c r="AJ3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="76" t="s">
+      <c r="AK3" s="92"/>
+      <c r="AL3" s="92"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
-      <c r="AQ2" s="74"/>
+      <c r="AO3" s="92"/>
+      <c r="AP3" s="92"/>
+      <c r="AQ3" s="93"/>
     </row>
-    <row r="3" spans="1:43" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="70" t="s">
+    <row r="4" spans="1:43" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="73"/>
+      <c r="B4" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C4" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D4" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E4" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F4" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G4" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="69" t="s">
+      <c r="H4" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I4" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J4" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K4" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="L4" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="69" t="s">
+      <c r="M4" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N4" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="66" t="s">
+      <c r="O4" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="67" t="s">
+      <c r="P4" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q4" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="66" t="s">
+      <c r="R4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="65" t="s">
+      <c r="S4" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="64" t="s">
+      <c r="T4" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="65" t="s">
+      <c r="U4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="65" t="s">
+      <c r="V4" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="64" t="s">
+      <c r="W4" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="X3" s="59" t="s">
+      <c r="X4" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="61" t="s">
+      <c r="Y4" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="60" t="s">
+      <c r="Z4" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="AA3" s="59" t="s">
+      <c r="AA4" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="63" t="s">
+      <c r="AB4" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="61" t="s">
+      <c r="AC4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="61" t="s">
+      <c r="AD4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="AE3" s="62" t="s">
+      <c r="AE4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="61" t="s">
+      <c r="AF4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AG3" s="60" t="s">
+      <c r="AG4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="AH3" s="59" t="s">
+      <c r="AH4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="AI3" s="58" t="s">
+      <c r="AI4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="AJ3" s="57" t="s">
+      <c r="AJ4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="AK3" s="56" t="s">
+      <c r="AK4" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="AL3" s="56" t="s">
+      <c r="AL4" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="AM3" s="55" t="s">
+      <c r="AM4" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="AN3" s="57" t="s">
+      <c r="AN4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="AO3" s="56" t="s">
+      <c r="AO4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AP3" s="56" t="s">
+      <c r="AP4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="AQ3" s="55" t="s">
+      <c r="AQ4" s="55" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A4" s="54">
-        <v>101</v>
-      </c>
-      <c r="B4" s="53">
-        <v>0</v>
-      </c>
-      <c r="C4" s="51">
-        <v>6</v>
-      </c>
-      <c r="D4" s="50">
-        <v>6.9</v>
-      </c>
-      <c r="E4" s="52">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F4" s="50">
-        <v>7.3</v>
-      </c>
-      <c r="G4" s="52">
-        <v>6.6</v>
-      </c>
-      <c r="H4" s="50">
-        <v>5.6</v>
-      </c>
-      <c r="I4" s="51">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J4" s="50">
-        <v>5.4</v>
-      </c>
-      <c r="K4" s="49">
-        <v>6.6</v>
-      </c>
-      <c r="L4" s="49">
-        <v>5.9</v>
-      </c>
-      <c r="M4" s="49">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="N4" s="48">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O4" s="43">
-        <v>3484.7</v>
-      </c>
-      <c r="P4" s="42">
-        <v>0.314</v>
-      </c>
-      <c r="Q4" s="41">
-        <v>0.314</v>
-      </c>
-      <c r="R4" s="47">
-        <v>34.801666666666662</v>
-      </c>
-      <c r="S4" s="46">
-        <v>55.806000000000004</v>
-      </c>
-      <c r="T4" s="45">
-        <v>315.37</v>
-      </c>
-      <c r="U4" s="47">
-        <v>34.801666666666662</v>
-      </c>
-      <c r="V4" s="46">
-        <v>55.806000000000004</v>
-      </c>
-      <c r="W4" s="45">
-        <v>315.37</v>
-      </c>
-      <c r="X4" s="44">
-        <v>44.58</v>
-      </c>
-      <c r="Y4" s="39">
-        <v>11.573</v>
-      </c>
-      <c r="Z4" s="38">
-        <v>0.45</v>
-      </c>
-      <c r="AA4" s="40">
-        <v>331.51</v>
-      </c>
-      <c r="AB4" s="39">
-        <v>46.851999999999997</v>
-      </c>
-      <c r="AC4" s="39">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="AD4" s="39">
-        <v>3.2349999999999999</v>
-      </c>
-      <c r="AE4" s="39">
-        <v>9.8339999999999996</v>
-      </c>
-      <c r="AF4" s="39">
-        <v>65.474999999999994</v>
-      </c>
-      <c r="AG4" s="44">
-        <v>82.495999999999995</v>
-      </c>
-      <c r="AH4" s="40">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="38">
-        <v>101.05</v>
-      </c>
-      <c r="AJ4" s="43">
-        <v>2.58</v>
-      </c>
-      <c r="AK4" s="42">
-        <v>-1.9930000000000001</v>
-      </c>
-      <c r="AL4" s="42">
-        <v>48.978000000000002</v>
-      </c>
-      <c r="AM4" s="41">
-        <v>28.783000000000001</v>
-      </c>
-      <c r="AN4" s="40">
-        <v>7.3819999999999997</v>
-      </c>
-      <c r="AO4" s="39">
-        <v>-3.6080000000000001</v>
-      </c>
-      <c r="AP4" s="39">
-        <v>54.167000000000002</v>
-      </c>
-      <c r="AQ4" s="38">
-        <v>-27.201000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
-        <v>102</v>
-      </c>
-      <c r="B5" s="26">
+      <c r="A5" s="54">
+        <v>101</v>
+      </c>
+      <c r="B5" s="53">
         <v>0</v>
       </c>
-      <c r="C5" s="23">
-        <v>4.2</v>
-      </c>
-      <c r="D5" s="29">
-        <v>7.7</v>
-      </c>
-      <c r="E5" s="30">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F5" s="24">
-        <v>4.7</v>
-      </c>
-      <c r="G5" s="25">
-        <v>3.9</v>
-      </c>
-      <c r="H5" s="24">
-        <v>6.3</v>
-      </c>
-      <c r="I5" s="23">
-        <v>5.7</v>
-      </c>
-      <c r="J5" s="29">
-        <v>6.2</v>
-      </c>
-      <c r="K5" s="37">
-        <v>7.2</v>
-      </c>
-      <c r="L5" s="37">
+      <c r="C5" s="51">
+        <v>6</v>
+      </c>
+      <c r="D5" s="50">
+        <v>6.9</v>
+      </c>
+      <c r="E5" s="52">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F5" s="50">
+        <v>7.3</v>
+      </c>
+      <c r="G5" s="52">
+        <v>6.6</v>
+      </c>
+      <c r="H5" s="50">
+        <v>5.6</v>
+      </c>
+      <c r="I5" s="51">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M5" s="23">
-        <v>4.3</v>
-      </c>
-      <c r="N5" s="28">
+      <c r="J5" s="50">
+        <v>5.4</v>
+      </c>
+      <c r="K5" s="49">
+        <v>6.6</v>
+      </c>
+      <c r="L5" s="49">
+        <v>5.9</v>
+      </c>
+      <c r="M5" s="49">
         <v>4.0999999999999996</v>
       </c>
-      <c r="O5" s="17">
-        <v>5476.25</v>
-      </c>
-      <c r="P5" s="16">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="Q5" s="15">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="R5" s="21">
-        <v>55.916666666666664</v>
-      </c>
-      <c r="S5" s="20">
-        <v>76.270666666666671</v>
-      </c>
-      <c r="T5" s="19">
-        <v>370.08333333333331</v>
-      </c>
-      <c r="U5" s="21">
-        <v>55.916666666666664</v>
-      </c>
-      <c r="V5" s="20">
-        <v>76.270666666666671</v>
-      </c>
-      <c r="W5" s="19">
-        <v>370.08333333333331</v>
-      </c>
-      <c r="X5" s="18">
-        <v>66.400999999999996</v>
-      </c>
-      <c r="Y5" s="16">
-        <v>7.0010000000000003</v>
-      </c>
-      <c r="Z5" s="15">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="AA5" s="17">
-        <v>4148.25</v>
-      </c>
-      <c r="AB5" s="16">
-        <v>1090.05</v>
-      </c>
-      <c r="AC5" s="16">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="AD5" s="16">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="AE5" s="16">
-        <v>22.68</v>
-      </c>
-      <c r="AF5" s="16">
-        <v>93.995000000000005</v>
-      </c>
-      <c r="AG5" s="18">
-        <v>51.991999999999997</v>
-      </c>
-      <c r="AH5" s="17">
-        <v>48.05</v>
-      </c>
-      <c r="AI5" s="15">
-        <v>61.7</v>
-      </c>
-      <c r="AJ5" s="17">
-        <v>4.9470000000000001</v>
-      </c>
-      <c r="AK5" s="16">
-        <v>-4.21</v>
-      </c>
-      <c r="AL5" s="16">
-        <v>96.218999999999994</v>
-      </c>
-      <c r="AM5" s="15">
-        <v>61.941000000000003</v>
-      </c>
-      <c r="AN5" s="17">
-        <v>21.111999999999998</v>
-      </c>
-      <c r="AO5" s="16">
-        <v>-9.1270000000000007</v>
-      </c>
-      <c r="AP5" s="16">
-        <v>143.24799999999999</v>
-      </c>
-      <c r="AQ5" s="15">
-        <v>-68.125</v>
+      <c r="N5" s="48">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O5" s="43">
+        <v>3484.7</v>
+      </c>
+      <c r="P5" s="42">
+        <v>0.314</v>
+      </c>
+      <c r="Q5" s="41">
+        <v>0.314</v>
+      </c>
+      <c r="R5" s="47">
+        <v>34.801666666666662</v>
+      </c>
+      <c r="S5" s="46">
+        <v>55.806000000000004</v>
+      </c>
+      <c r="T5" s="45">
+        <v>315.37</v>
+      </c>
+      <c r="U5" s="47">
+        <v>34.801666666666662</v>
+      </c>
+      <c r="V5" s="46">
+        <v>55.806000000000004</v>
+      </c>
+      <c r="W5" s="45">
+        <v>315.37</v>
+      </c>
+      <c r="X5" s="44">
+        <v>44.58</v>
+      </c>
+      <c r="Y5" s="39">
+        <v>11.573</v>
+      </c>
+      <c r="Z5" s="38">
+        <v>0.45</v>
+      </c>
+      <c r="AA5" s="40">
+        <v>331.51</v>
+      </c>
+      <c r="AB5" s="39">
+        <v>46.851999999999997</v>
+      </c>
+      <c r="AC5" s="39">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AD5" s="39">
+        <v>3.2349999999999999</v>
+      </c>
+      <c r="AE5" s="39">
+        <v>9.8339999999999996</v>
+      </c>
+      <c r="AF5" s="39">
+        <v>65.474999999999994</v>
+      </c>
+      <c r="AG5" s="44">
+        <v>82.495999999999995</v>
+      </c>
+      <c r="AH5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="38">
+        <v>101.05</v>
+      </c>
+      <c r="AJ5" s="43">
+        <v>2.58</v>
+      </c>
+      <c r="AK5" s="42">
+        <v>-1.9930000000000001</v>
+      </c>
+      <c r="AL5" s="42">
+        <v>48.978000000000002</v>
+      </c>
+      <c r="AM5" s="41">
+        <v>28.783000000000001</v>
+      </c>
+      <c r="AN5" s="40">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="AO5" s="39">
+        <v>-3.6080000000000001</v>
+      </c>
+      <c r="AP5" s="39">
+        <v>54.167000000000002</v>
+      </c>
+      <c r="AQ5" s="38">
+        <v>-27.201000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="27">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="26">
         <v>0</v>
       </c>
       <c r="C6" s="23">
-        <v>5.8</v>
+        <v>4.2</v>
       </c>
       <c r="D6" s="29">
-        <v>5.9</v>
+        <v>7.7</v>
       </c>
       <c r="E6" s="30">
-        <v>3.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F6" s="24">
-        <v>5.8</v>
+        <v>4.7</v>
       </c>
       <c r="G6" s="25">
+        <v>3.9</v>
+      </c>
+      <c r="H6" s="24">
         <v>6.3</v>
       </c>
-      <c r="H6" s="24">
-        <v>5.8</v>
-      </c>
       <c r="I6" s="23">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
       <c r="J6" s="29">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="K6" s="37">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="L6" s="37">
-        <v>6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="M6" s="23">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="N6" s="28">
         <v>4.0999999999999996</v>
       </c>
       <c r="O6" s="17">
-        <v>3339.15</v>
+        <v>5476.25</v>
       </c>
       <c r="P6" s="16">
-        <v>0.38600000000000001</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="Q6" s="15">
-        <v>0.38600000000000001</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="R6" s="21">
-        <v>79.259666666666661</v>
+        <v>55.916666666666664</v>
       </c>
       <c r="S6" s="20">
-        <v>98.826666666666668</v>
+        <v>76.270666666666671</v>
       </c>
       <c r="T6" s="19">
-        <v>423.57333333333332</v>
+        <v>370.08333333333331</v>
       </c>
       <c r="U6" s="21">
-        <v>79.259666666666661</v>
+        <v>55.916666666666664</v>
       </c>
       <c r="V6" s="20">
-        <v>98.826666666666668</v>
+        <v>76.270666666666671</v>
       </c>
       <c r="W6" s="19">
-        <v>423.57333333333332</v>
+        <v>370.08333333333331</v>
       </c>
       <c r="X6" s="18">
-        <v>31.343</v>
+        <v>66.400999999999996</v>
       </c>
       <c r="Y6" s="16">
-        <v>25.521000000000001</v>
+        <v>7.0010000000000003</v>
       </c>
       <c r="Z6" s="15">
-        <v>0.35799999999999998</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="AA6" s="17">
-        <v>336.57499999999999</v>
+        <v>4148.25</v>
       </c>
       <c r="AB6" s="16">
-        <v>43.912999999999997</v>
+        <v>1090.05</v>
       </c>
       <c r="AC6" s="16">
-        <v>0.13</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="AD6" s="16">
-        <v>4.2350000000000003</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="AE6" s="16">
-        <v>14.031000000000001</v>
+        <v>22.68</v>
       </c>
       <c r="AF6" s="16">
-        <v>77.144999999999996</v>
+        <v>93.995000000000005</v>
       </c>
       <c r="AG6" s="18">
-        <v>67.046000000000006</v>
+        <v>51.991999999999997</v>
       </c>
       <c r="AH6" s="17">
-        <v>93.7</v>
+        <v>48.05</v>
       </c>
       <c r="AI6" s="15">
-        <v>105.2</v>
+        <v>61.7</v>
       </c>
       <c r="AJ6" s="17">
-        <v>2.907</v>
+        <v>4.9470000000000001</v>
       </c>
       <c r="AK6" s="16">
-        <v>-2.363</v>
+        <v>-4.21</v>
       </c>
       <c r="AL6" s="16">
-        <v>61.237000000000002</v>
+        <v>96.218999999999994</v>
       </c>
       <c r="AM6" s="15">
-        <v>35.213000000000001</v>
+        <v>61.941000000000003</v>
       </c>
       <c r="AN6" s="17">
-        <v>8.1289999999999996</v>
+        <v>21.111999999999998</v>
       </c>
       <c r="AO6" s="16">
-        <v>-3.29</v>
+        <v>-9.1270000000000007</v>
       </c>
       <c r="AP6" s="16">
-        <v>59.67</v>
+        <v>143.24799999999999</v>
       </c>
       <c r="AQ6" s="15">
-        <v>-24.241</v>
+        <v>-68.125</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="27">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
       </c>
       <c r="C7" s="23">
+        <v>5.8</v>
+      </c>
+      <c r="D7" s="29">
         <v>5.9</v>
       </c>
-      <c r="D7" s="36">
+      <c r="E7" s="30">
+        <v>3.1</v>
+      </c>
+      <c r="F7" s="24">
         <v>5.8</v>
       </c>
-      <c r="E7" s="30">
-        <v>9.1</v>
-      </c>
-      <c r="F7" s="24">
-        <v>6.7</v>
-      </c>
       <c r="G7" s="25">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="H7" s="24">
+        <v>5.8</v>
+      </c>
+      <c r="I7" s="23">
+        <v>5.4</v>
+      </c>
+      <c r="J7" s="29">
+        <v>5.3</v>
+      </c>
+      <c r="K7" s="37">
+        <v>7.3</v>
+      </c>
+      <c r="L7" s="37">
         <v>6</v>
       </c>
-      <c r="I7" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="J7" s="36">
-        <v>6.6</v>
-      </c>
-      <c r="K7" s="35">
-        <v>7.2</v>
-      </c>
-      <c r="L7" s="35">
-        <v>3.1</v>
-      </c>
-      <c r="M7" s="35">
-        <v>4.2</v>
-      </c>
-      <c r="N7" s="34">
-        <v>6.1</v>
+      <c r="M7" s="23">
+        <v>4</v>
+      </c>
+      <c r="N7" s="28">
+        <v>4.0999999999999996</v>
       </c>
       <c r="O7" s="17">
-        <v>3479.5</v>
+        <v>3339.15</v>
       </c>
       <c r="P7" s="16">
-        <v>0.41399999999999998</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="Q7" s="15">
-        <v>0.41399999999999998</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="R7" s="21">
-        <v>101.48966666666666</v>
+        <v>79.259666666666661</v>
       </c>
       <c r="S7" s="20">
-        <v>120.33999999999999</v>
+        <v>98.826666666666668</v>
       </c>
       <c r="T7" s="19">
-        <v>477.67333333333335</v>
+        <v>423.57333333333332</v>
       </c>
       <c r="U7" s="21">
-        <v>101.48966666666666</v>
+        <v>79.259666666666661</v>
       </c>
       <c r="V7" s="20">
-        <v>120.33999999999999</v>
+        <v>98.826666666666668</v>
       </c>
       <c r="W7" s="19">
-        <v>477.67333333333335</v>
+        <v>423.57333333333332</v>
       </c>
       <c r="X7" s="18">
-        <v>68.596000000000004</v>
+        <v>31.343</v>
       </c>
       <c r="Y7" s="16">
-        <v>11.397</v>
+        <v>25.521000000000001</v>
       </c>
       <c r="Z7" s="15">
-        <v>0.502</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="AA7" s="17">
-        <v>345.125</v>
+        <v>336.57499999999999</v>
       </c>
       <c r="AB7" s="16">
-        <v>64.561000000000007</v>
+        <v>43.912999999999997</v>
       </c>
       <c r="AC7" s="16">
-        <v>0.187</v>
+        <v>0.13</v>
       </c>
       <c r="AD7" s="16">
-        <v>3.91</v>
+        <v>4.2350000000000003</v>
       </c>
       <c r="AE7" s="16">
-        <v>12.547000000000001</v>
+        <v>14.031000000000001</v>
       </c>
       <c r="AF7" s="16">
-        <v>103.2</v>
+        <v>77.144999999999996</v>
       </c>
       <c r="AG7" s="18">
-        <v>111.715</v>
+        <v>67.046000000000006</v>
       </c>
       <c r="AH7" s="17">
-        <v>50.9</v>
+        <v>93.7</v>
       </c>
       <c r="AI7" s="15">
-        <v>69.45</v>
+        <v>105.2</v>
       </c>
       <c r="AJ7" s="17">
-        <v>4.7370000000000001</v>
+        <v>2.907</v>
       </c>
       <c r="AK7" s="16">
-        <v>-3.3170000000000002</v>
+        <v>-2.363</v>
       </c>
       <c r="AL7" s="16">
-        <v>91.168999999999997</v>
+        <v>61.237000000000002</v>
       </c>
       <c r="AM7" s="15">
-        <v>44.000999999999998</v>
+        <v>35.213000000000001</v>
       </c>
       <c r="AN7" s="17">
-        <v>14.974</v>
+        <v>8.1289999999999996</v>
       </c>
       <c r="AO7" s="16">
-        <v>-3.069</v>
+        <v>-3.29</v>
       </c>
       <c r="AP7" s="16">
-        <v>108.63800000000001</v>
+        <v>59.67</v>
       </c>
       <c r="AQ7" s="15">
-        <v>-17.844000000000001</v>
+        <v>-24.241</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="27">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="26">
         <v>0</v>
       </c>
       <c r="C8" s="23">
+        <v>5.9</v>
+      </c>
+      <c r="D8" s="36">
+        <v>5.8</v>
+      </c>
+      <c r="E8" s="30">
+        <v>9.1</v>
+      </c>
+      <c r="F8" s="24">
+        <v>6.7</v>
+      </c>
+      <c r="G8" s="25">
+        <v>6.5</v>
+      </c>
+      <c r="H8" s="24">
+        <v>6</v>
+      </c>
+      <c r="I8" s="23">
         <v>5.2</v>
       </c>
-      <c r="D8" s="24">
-        <v>8</v>
-      </c>
-      <c r="E8" s="25">
-        <v>3.4</v>
-      </c>
-      <c r="F8" s="24">
+      <c r="J8" s="36">
+        <v>6.6</v>
+      </c>
+      <c r="K8" s="35">
+        <v>7.2</v>
+      </c>
+      <c r="L8" s="35">
+        <v>3.1</v>
+      </c>
+      <c r="M8" s="35">
+        <v>4.2</v>
+      </c>
+      <c r="N8" s="34">
         <v>6.1</v>
       </c>
-      <c r="G8" s="25">
-        <v>6.2</v>
-      </c>
-      <c r="H8" s="24">
-        <v>7</v>
-      </c>
-      <c r="I8" s="23">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J8" s="33">
-        <v>3.2</v>
-      </c>
-      <c r="K8" s="23">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="L8" s="23">
-        <v>5.8</v>
-      </c>
-      <c r="M8" s="23">
-        <v>2.8</v>
-      </c>
-      <c r="N8" s="32">
-        <v>1.9</v>
-      </c>
       <c r="O8" s="17">
-        <v>833.14</v>
+        <v>3479.5</v>
       </c>
       <c r="P8" s="16">
-        <v>0.32200000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="Q8" s="15">
-        <v>0.32200000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="R8" s="21">
-        <v>80.060666666666663</v>
+        <v>101.48966666666666</v>
       </c>
       <c r="S8" s="20">
-        <v>100.27366666666667</v>
+        <v>120.33999999999999</v>
       </c>
       <c r="T8" s="19">
-        <v>447.08333333333331</v>
+        <v>477.67333333333335</v>
       </c>
       <c r="U8" s="21">
-        <v>80.060666666666663</v>
+        <v>101.48966666666666</v>
       </c>
       <c r="V8" s="20">
-        <v>100.27366666666667</v>
+        <v>120.33999999999999</v>
       </c>
       <c r="W8" s="19">
-        <v>447.08333333333331</v>
+        <v>477.67333333333335</v>
       </c>
       <c r="X8" s="18">
-        <v>9.8040000000000003</v>
+        <v>68.596000000000004</v>
       </c>
       <c r="Y8" s="16">
-        <v>4.8499999999999996</v>
+        <v>11.397</v>
       </c>
       <c r="Z8" s="15">
-        <v>0.876</v>
+        <v>0.502</v>
       </c>
       <c r="AA8" s="17">
-        <v>3111.9</v>
+        <v>345.125</v>
       </c>
       <c r="AB8" s="16">
-        <v>873.48</v>
+        <v>64.561000000000007</v>
       </c>
       <c r="AC8" s="16">
-        <v>0.28100000000000003</v>
+        <v>0.187</v>
       </c>
       <c r="AD8" s="16">
-        <v>6.9000000000000006E-2</v>
+        <v>3.91</v>
       </c>
       <c r="AE8" s="16">
-        <v>1.9910000000000001</v>
+        <v>12.547000000000001</v>
       </c>
       <c r="AF8" s="16">
-        <v>84.784999999999997</v>
+        <v>103.2</v>
       </c>
       <c r="AG8" s="18">
-        <v>42.295999999999999</v>
+        <v>111.715</v>
       </c>
       <c r="AH8" s="17">
-        <v>0</v>
+        <v>50.9</v>
       </c>
       <c r="AI8" s="15">
-        <v>23.85</v>
+        <v>69.45</v>
       </c>
       <c r="AJ8" s="17">
-        <v>4.8099999999999996</v>
+        <v>4.7370000000000001</v>
       </c>
       <c r="AK8" s="16">
-        <v>-3.7970000000000002</v>
+        <v>-3.3170000000000002</v>
       </c>
       <c r="AL8" s="16">
-        <v>90.253</v>
+        <v>91.168999999999997</v>
       </c>
       <c r="AM8" s="15">
-        <v>51.378</v>
+        <v>44.000999999999998</v>
       </c>
       <c r="AN8" s="17">
-        <v>19.131</v>
+        <v>14.974</v>
       </c>
       <c r="AO8" s="16">
-        <v>-8.7260000000000009</v>
+        <v>-3.069</v>
       </c>
       <c r="AP8" s="16">
-        <v>143.286</v>
+        <v>108.63800000000001</v>
       </c>
       <c r="AQ8" s="15">
-        <v>-56.201999999999998</v>
+        <v>-17.844000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A9" s="31">
-        <v>106</v>
+      <c r="A9" s="27">
+        <v>105</v>
       </c>
       <c r="B9" s="26">
         <v>0</v>
       </c>
       <c r="C9" s="23">
-        <v>3.6</v>
-      </c>
-      <c r="D9" s="29">
-        <v>7.8</v>
-      </c>
-      <c r="E9" s="30">
-        <v>8.1999999999999993</v>
+        <v>5.2</v>
+      </c>
+      <c r="D9" s="24">
+        <v>8</v>
+      </c>
+      <c r="E9" s="25">
+        <v>3.4</v>
       </c>
       <c r="F9" s="24">
-        <v>3.5</v>
+        <v>6.1</v>
       </c>
       <c r="G9" s="25">
-        <v>3.3</v>
+        <v>6.2</v>
       </c>
       <c r="H9" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I9" s="23">
-        <v>6.4</v>
-      </c>
-      <c r="J9" s="29">
-        <v>6.1</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J9" s="33">
+        <v>3.2</v>
       </c>
       <c r="K9" s="23">
-        <v>6.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="L9" s="23">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
       <c r="M9" s="23">
-        <v>5.2</v>
-      </c>
-      <c r="N9" s="28">
-        <v>4.0999999999999996</v>
+        <v>2.8</v>
+      </c>
+      <c r="N9" s="32">
+        <v>1.9</v>
       </c>
       <c r="O9" s="17">
-        <v>1532.75</v>
+        <v>833.14</v>
       </c>
       <c r="P9" s="16">
-        <v>0.504</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="Q9" s="15">
-        <v>0.504</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="R9" s="21">
-        <v>56.074333333333335</v>
+        <v>80.060666666666663</v>
       </c>
       <c r="S9" s="20">
-        <v>78.012</v>
+        <v>100.27366666666667</v>
       </c>
       <c r="T9" s="19">
-        <v>417.57333333333332</v>
+        <v>447.08333333333331</v>
       </c>
       <c r="U9" s="21">
-        <v>56.074333333333335</v>
+        <v>80.060666666666663</v>
       </c>
       <c r="V9" s="20">
-        <v>78.012</v>
+        <v>100.27366666666667</v>
       </c>
       <c r="W9" s="19">
-        <v>417.57333333333332</v>
+        <v>447.08333333333331</v>
       </c>
       <c r="X9" s="18">
-        <v>28.992000000000001</v>
+        <v>9.8040000000000003</v>
       </c>
       <c r="Y9" s="16">
-        <v>9.3829999999999991</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="Z9" s="15">
-        <v>0.50600000000000001</v>
+        <v>0.876</v>
       </c>
       <c r="AA9" s="17">
-        <v>2111.25</v>
+        <v>3111.9</v>
       </c>
       <c r="AB9" s="16">
-        <v>481.78500000000003</v>
+        <v>873.48</v>
       </c>
       <c r="AC9" s="16">
-        <v>0.22900000000000001</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="AD9" s="16">
-        <v>0.81799999999999995</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="AE9" s="16">
-        <v>16.724</v>
+        <v>1.9910000000000001</v>
       </c>
       <c r="AF9" s="16">
-        <v>77.344999999999999</v>
+        <v>84.784999999999997</v>
       </c>
       <c r="AG9" s="18">
-        <v>32.35</v>
+        <v>42.295999999999999</v>
       </c>
       <c r="AH9" s="17">
-        <v>20.5</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="15">
-        <v>32.35</v>
+        <v>23.85</v>
       </c>
       <c r="AJ9" s="17">
-        <v>4.0129999999999999</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="AK9" s="16">
-        <v>-3.54</v>
+        <v>-3.7970000000000002</v>
       </c>
       <c r="AL9" s="16">
-        <v>83.656000000000006</v>
+        <v>90.253</v>
       </c>
       <c r="AM9" s="15">
-        <v>52.393000000000001</v>
+        <v>51.378</v>
       </c>
       <c r="AN9" s="17">
-        <v>17.641999999999999</v>
+        <v>19.131</v>
       </c>
       <c r="AO9" s="16">
-        <v>-8.0730000000000004</v>
+        <v>-8.7260000000000009</v>
       </c>
       <c r="AP9" s="16">
-        <v>133.19399999999999</v>
+        <v>143.286</v>
       </c>
       <c r="AQ9" s="15">
-        <v>-58.287999999999997</v>
+        <v>-56.201999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <v>107</v>
+      <c r="A10" s="31">
+        <v>106</v>
       </c>
       <c r="B10" s="26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="23">
-        <v>3.7</v>
-      </c>
-      <c r="D10" s="24">
-        <v>3.7</v>
+        <v>3.6</v>
+      </c>
+      <c r="D10" s="29">
+        <v>7.8</v>
       </c>
       <c r="E10" s="30">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F10" s="24">
         <v>3.5</v>
       </c>
-      <c r="F10" s="24">
-        <v>5.0999999999999996</v>
-      </c>
       <c r="G10" s="25">
-        <v>5.8</v>
+        <v>3.3</v>
       </c>
       <c r="H10" s="24">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="I10" s="23">
-        <v>4.5999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="J10" s="29">
-        <v>4.9000000000000004</v>
+        <v>6.1</v>
       </c>
       <c r="K10" s="23">
-        <v>7.6</v>
+        <v>6.6</v>
       </c>
       <c r="L10" s="23">
         <v>5.5</v>
       </c>
       <c r="M10" s="23">
-        <v>3.3</v>
+        <v>5.2</v>
       </c>
       <c r="N10" s="28">
-        <v>3.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O10" s="17">
-        <v>7349.25</v>
+        <v>1532.75</v>
       </c>
       <c r="P10" s="16">
-        <v>0.502</v>
+        <v>0.504</v>
       </c>
       <c r="Q10" s="15">
-        <v>0.502</v>
+        <v>0.504</v>
       </c>
       <c r="R10" s="21">
-        <v>33.249000000000002</v>
+        <v>56.074333333333335</v>
       </c>
       <c r="S10" s="20">
-        <v>57.347666666666669</v>
+        <v>78.012</v>
       </c>
       <c r="T10" s="19">
-        <v>385.72666666666663</v>
+        <v>417.57333333333332</v>
       </c>
       <c r="U10" s="21">
-        <v>33.249000000000002</v>
+        <v>56.074333333333335</v>
       </c>
       <c r="V10" s="20">
-        <v>57.347666666666669</v>
+        <v>78.012</v>
       </c>
       <c r="W10" s="19">
-        <v>385.72666666666663</v>
+        <v>417.57333333333332</v>
       </c>
       <c r="X10" s="18">
-        <v>99.128</v>
+        <v>28.992000000000001</v>
       </c>
       <c r="Y10" s="16">
-        <v>23.097999999999999</v>
+        <v>9.3829999999999991</v>
       </c>
       <c r="Z10" s="15">
-        <v>0.39500000000000002</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="AA10" s="17">
-        <v>1179</v>
+        <v>2111.25</v>
       </c>
       <c r="AB10" s="16">
-        <v>114.44499999999999</v>
+        <v>481.78500000000003</v>
       </c>
       <c r="AC10" s="16">
-        <v>9.7000000000000003E-2</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="AD10" s="16">
-        <v>2.89</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="AE10" s="16">
-        <v>32.19</v>
+        <v>16.724</v>
       </c>
       <c r="AF10" s="16">
-        <v>159</v>
+        <v>77.344999999999999</v>
       </c>
       <c r="AG10" s="18">
-        <v>58.180999999999997</v>
+        <v>32.35</v>
       </c>
       <c r="AH10" s="17">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="AI10" s="15">
-        <v>83.6</v>
+        <v>32.35</v>
       </c>
       <c r="AJ10" s="17">
-        <v>5.3869999999999996</v>
+        <v>4.0129999999999999</v>
       </c>
       <c r="AK10" s="16">
-        <v>-4.6500000000000004</v>
+        <v>-3.54</v>
       </c>
       <c r="AL10" s="16">
-        <v>109.17700000000001</v>
+        <v>83.656000000000006</v>
       </c>
       <c r="AM10" s="15">
-        <v>72.322999999999993</v>
+        <v>52.393000000000001</v>
       </c>
       <c r="AN10" s="17">
-        <v>15.95</v>
+        <v>17.641999999999999</v>
       </c>
       <c r="AO10" s="16">
-        <v>-8.5510000000000002</v>
+        <v>-8.0730000000000004</v>
       </c>
       <c r="AP10" s="16">
-        <v>111.35899999999999</v>
+        <v>133.19399999999999</v>
       </c>
       <c r="AQ10" s="15">
-        <v>-64.668999999999997</v>
+        <v>-58.287999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" s="27">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="23">
+        <v>3.7</v>
+      </c>
+      <c r="D11" s="24">
+        <v>3.7</v>
+      </c>
+      <c r="E11" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G11" s="25">
+        <v>5.8</v>
+      </c>
+      <c r="H11" s="24">
+        <v>5.7</v>
+      </c>
+      <c r="I11" s="23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J11" s="29">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K11" s="23">
+        <v>7.6</v>
+      </c>
+      <c r="L11" s="23">
+        <v>5.5</v>
+      </c>
+      <c r="M11" s="23">
+        <v>3.3</v>
+      </c>
+      <c r="N11" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="O11" s="17">
+        <v>7349.25</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.502</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>0.502</v>
+      </c>
+      <c r="R11" s="21">
+        <v>33.249000000000002</v>
+      </c>
+      <c r="S11" s="20">
+        <v>57.347666666666669</v>
+      </c>
+      <c r="T11" s="19">
+        <v>385.72666666666663</v>
+      </c>
+      <c r="U11" s="21">
+        <v>33.249000000000002</v>
+      </c>
+      <c r="V11" s="20">
+        <v>57.347666666666669</v>
+      </c>
+      <c r="W11" s="19">
+        <v>385.72666666666663</v>
+      </c>
+      <c r="X11" s="18">
+        <v>99.128</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>23.097999999999999</v>
+      </c>
+      <c r="Z11" s="15">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>1179</v>
+      </c>
+      <c r="AB11" s="16">
+        <v>114.44499999999999</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AD11" s="16">
+        <v>2.89</v>
+      </c>
+      <c r="AE11" s="16">
+        <v>32.19</v>
+      </c>
+      <c r="AF11" s="16">
+        <v>159</v>
+      </c>
+      <c r="AG11" s="18">
+        <v>58.180999999999997</v>
+      </c>
+      <c r="AH11" s="17">
         <v>0</v>
       </c>
-      <c r="C11" s="23">
-        <v>3</v>
-      </c>
-      <c r="D11" s="29">
-        <v>8</v>
-      </c>
-      <c r="E11" s="30">
-        <v>6</v>
-      </c>
-      <c r="F11" s="24">
-        <v>4</v>
-      </c>
-      <c r="G11" s="25">
-        <v>4</v>
-      </c>
-      <c r="H11" s="24">
-        <v>4</v>
-      </c>
-      <c r="I11" s="23">
-        <v>7</v>
-      </c>
-      <c r="J11" s="24">
-        <v>8</v>
-      </c>
-      <c r="K11" s="23">
-        <v>4</v>
-      </c>
-      <c r="L11" s="23">
-        <v>4</v>
-      </c>
-      <c r="M11" s="23">
-        <v>7</v>
-      </c>
-      <c r="N11" s="28">
-        <v>7</v>
-      </c>
-      <c r="O11" s="17">
-        <v>772.65499999999997</v>
-      </c>
-      <c r="P11" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="Q11" s="15">
-        <v>0.33</v>
-      </c>
-      <c r="R11" s="21">
-        <v>33.805666666666667</v>
-      </c>
-      <c r="S11" s="20">
-        <v>65.132000000000005</v>
-      </c>
-      <c r="T11" s="19">
-        <v>397.88666666666671</v>
-      </c>
-      <c r="U11" s="21">
-        <v>33.805666666666667</v>
-      </c>
-      <c r="V11" s="20">
-        <v>65.132000000000005</v>
-      </c>
-      <c r="W11" s="19">
-        <v>397.88666666666671</v>
-      </c>
-      <c r="X11" s="18">
-        <v>23.338000000000001</v>
-      </c>
-      <c r="Y11" s="16">
-        <v>2.2719999999999998</v>
-      </c>
-      <c r="Z11" s="15">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="AA11" s="17">
-        <v>3078.9</v>
-      </c>
-      <c r="AB11" s="16">
-        <v>738.19</v>
-      </c>
-      <c r="AC11" s="16">
-        <v>0.24</v>
-      </c>
-      <c r="AD11" s="16">
-        <v>0.44</v>
-      </c>
-      <c r="AE11" s="16">
-        <v>12.925000000000001</v>
-      </c>
-      <c r="AF11" s="16">
-        <v>57.034999999999997</v>
-      </c>
-      <c r="AG11" s="18">
-        <v>33.335999999999999</v>
-      </c>
-      <c r="AH11" s="17">
-        <v>13.65</v>
-      </c>
       <c r="AI11" s="15">
-        <v>24.25</v>
+        <v>83.6</v>
       </c>
       <c r="AJ11" s="17">
-        <v>3.5030000000000001</v>
+        <v>5.3869999999999996</v>
       </c>
       <c r="AK11" s="16">
-        <v>-2.92</v>
+        <v>-4.6500000000000004</v>
       </c>
       <c r="AL11" s="16">
-        <v>72.103999999999999</v>
+        <v>109.17700000000001</v>
       </c>
       <c r="AM11" s="15">
-        <v>40.771000000000001</v>
+        <v>72.322999999999993</v>
       </c>
       <c r="AN11" s="17">
-        <v>13.013999999999999</v>
+        <v>15.95</v>
       </c>
       <c r="AO11" s="16">
-        <v>-5.9939999999999998</v>
+        <v>-8.5510000000000002</v>
       </c>
       <c r="AP11" s="16">
-        <v>91.56</v>
+        <v>111.35899999999999</v>
       </c>
       <c r="AQ11" s="15">
-        <v>-44.262</v>
+        <v>-64.668999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="27">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C12" s="23">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29">
+        <v>8</v>
+      </c>
+      <c r="E12" s="30">
+        <v>6</v>
+      </c>
+      <c r="F12" s="24">
+        <v>4</v>
+      </c>
+      <c r="G12" s="25">
+        <v>4</v>
+      </c>
+      <c r="H12" s="24">
+        <v>4</v>
+      </c>
+      <c r="I12" s="23">
         <v>7</v>
       </c>
-      <c r="D12" s="29">
-        <v>8.5</v>
-      </c>
-      <c r="E12" s="30">
+      <c r="J12" s="24">
+        <v>8</v>
+      </c>
+      <c r="K12" s="23">
+        <v>4</v>
+      </c>
+      <c r="L12" s="23">
+        <v>4</v>
+      </c>
+      <c r="M12" s="23">
         <v>7</v>
       </c>
-      <c r="F12" s="29">
-        <v>6</v>
-      </c>
-      <c r="G12" s="25">
-        <v>5</v>
-      </c>
-      <c r="H12" s="24">
-        <v>3</v>
-      </c>
-      <c r="I12" s="23">
-        <v>3</v>
-      </c>
-      <c r="J12" s="29">
-        <v>6</v>
-      </c>
-      <c r="K12" s="23">
-        <v>2</v>
-      </c>
-      <c r="L12" s="23">
+      <c r="N12" s="28">
         <v>7</v>
       </c>
-      <c r="M12" s="23">
-        <v>8</v>
-      </c>
-      <c r="N12" s="28">
-        <v>6</v>
-      </c>
       <c r="O12" s="17">
-        <v>55.808</v>
+        <v>772.65499999999997</v>
       </c>
       <c r="P12" s="16">
-        <v>0.49199999999999999</v>
+        <v>0.33</v>
       </c>
       <c r="Q12" s="15">
-        <v>0.49199999999999999</v>
+        <v>0.33</v>
       </c>
       <c r="R12" s="21">
-        <v>34.18266666666667</v>
+        <v>33.805666666666667</v>
       </c>
       <c r="S12" s="20">
-        <v>72.348666666666674</v>
+        <v>65.132000000000005</v>
       </c>
       <c r="T12" s="19">
-        <v>404.48999999999995</v>
+        <v>397.88666666666671</v>
       </c>
       <c r="U12" s="21">
-        <v>34.18266666666667</v>
+        <v>33.805666666666667</v>
       </c>
       <c r="V12" s="20">
-        <v>72.348666666666674</v>
+        <v>65.132000000000005</v>
       </c>
       <c r="W12" s="19">
-        <v>404.48999999999995</v>
+        <v>397.88666666666671</v>
       </c>
       <c r="X12" s="18">
-        <v>0.40200000000000002</v>
+        <v>23.338000000000001</v>
       </c>
       <c r="Y12" s="16">
-        <v>5.5369999999999999</v>
+        <v>2.2719999999999998</v>
       </c>
       <c r="Z12" s="15">
-        <v>0.66500000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="AA12" s="17">
-        <v>39.654000000000003</v>
+        <v>3078.9</v>
       </c>
       <c r="AB12" s="16">
-        <v>27.792000000000002</v>
+        <v>738.19</v>
       </c>
       <c r="AC12" s="16">
-        <v>0.70099999999999996</v>
+        <v>0.24</v>
       </c>
       <c r="AD12" s="16">
-        <v>1.615</v>
+        <v>0.44</v>
       </c>
       <c r="AE12" s="16">
-        <v>0.72099999999999997</v>
+        <v>12.925000000000001</v>
       </c>
       <c r="AF12" s="16">
-        <v>2.3860000000000001</v>
+        <v>57.034999999999997</v>
       </c>
       <c r="AG12" s="18">
-        <v>7.0579999999999998</v>
+        <v>33.335999999999999</v>
       </c>
       <c r="AH12" s="17">
-        <v>85.45</v>
+        <v>13.65</v>
       </c>
       <c r="AI12" s="15">
-        <v>83.75</v>
+        <v>24.25</v>
       </c>
       <c r="AJ12" s="17">
-        <v>0.69</v>
+        <v>3.5030000000000001</v>
       </c>
       <c r="AK12" s="16">
-        <v>-0.45500000000000002</v>
+        <v>-2.92</v>
       </c>
       <c r="AL12" s="16">
-        <v>12.882</v>
+        <v>72.103999999999999</v>
       </c>
       <c r="AM12" s="15">
-        <v>8.35</v>
+        <v>40.771000000000001</v>
       </c>
       <c r="AN12" s="17">
-        <v>1.7509999999999999</v>
+        <v>13.013999999999999</v>
       </c>
       <c r="AO12" s="16">
-        <v>-0.77600000000000002</v>
+        <v>-5.9939999999999998</v>
       </c>
       <c r="AP12" s="16">
-        <v>19.751000000000001</v>
+        <v>91.56</v>
       </c>
       <c r="AQ12" s="15">
-        <v>-6.0259999999999998</v>
+        <v>-44.262</v>
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C13" s="23">
-        <v>5.7</v>
+        <v>7</v>
       </c>
       <c r="D13" s="29">
-        <v>8.1999999999999993</v>
+        <v>8.5</v>
       </c>
       <c r="E13" s="30">
-        <v>9.1</v>
-      </c>
-      <c r="F13" s="24">
-        <v>6.5</v>
-      </c>
-      <c r="G13" s="30">
-        <v>6.9</v>
+        <v>7</v>
+      </c>
+      <c r="F13" s="29">
+        <v>6</v>
+      </c>
+      <c r="G13" s="25">
+        <v>5</v>
       </c>
       <c r="H13" s="24">
-        <v>4.5999999999999996</v>
+        <v>3</v>
       </c>
       <c r="I13" s="23">
-        <v>5.2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="29">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="K13" s="23">
+        <v>2</v>
+      </c>
+      <c r="L13" s="23">
+        <v>7</v>
+      </c>
+      <c r="M13" s="23">
+        <v>8</v>
+      </c>
+      <c r="N13" s="28">
         <v>6</v>
       </c>
-      <c r="L13" s="23">
-        <v>6.4</v>
-      </c>
-      <c r="M13" s="23">
-        <v>4.8</v>
-      </c>
-      <c r="N13" s="28">
-        <v>5.6</v>
-      </c>
       <c r="O13" s="17">
-        <v>2298.15</v>
+        <v>55.808</v>
       </c>
       <c r="P13" s="16">
-        <v>0.192</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="Q13" s="15">
-        <v>0.192</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="R13" s="21">
-        <v>34.764666666666663</v>
+        <v>34.18266666666667</v>
       </c>
       <c r="S13" s="20">
-        <v>77.349666666666664</v>
+        <v>72.348666666666674</v>
       </c>
       <c r="T13" s="19">
-        <v>415.67</v>
+        <v>404.48999999999995</v>
       </c>
       <c r="U13" s="21">
-        <v>34.764666666666663</v>
+        <v>34.18266666666667</v>
       </c>
       <c r="V13" s="20">
-        <v>77.349666666666664</v>
+        <v>72.348666666666674</v>
       </c>
       <c r="W13" s="19">
-        <v>415.67</v>
+        <v>404.48999999999995</v>
       </c>
       <c r="X13" s="18">
-        <v>27.05</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="Y13" s="16">
-        <v>4.0199999999999996</v>
+        <v>5.5369999999999999</v>
       </c>
       <c r="Z13" s="15">
-        <v>0.55500000000000005</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="AA13" s="17">
-        <v>676.67</v>
+        <v>39.654000000000003</v>
       </c>
       <c r="AB13" s="16">
-        <v>186.215</v>
+        <v>27.792000000000002</v>
       </c>
       <c r="AC13" s="16">
-        <v>0.27500000000000002</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="AD13" s="16">
-        <v>1.28</v>
+        <v>1.615</v>
       </c>
       <c r="AE13" s="16">
-        <v>7.6</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="AF13" s="16">
-        <v>33.344999999999999</v>
+        <v>2.3860000000000001</v>
       </c>
       <c r="AG13" s="18">
-        <v>43.427999999999997</v>
+        <v>7.0579999999999998</v>
       </c>
       <c r="AH13" s="17">
-        <v>0</v>
+        <v>85.45</v>
       </c>
       <c r="AI13" s="15">
-        <v>43.65</v>
+        <v>83.75</v>
       </c>
       <c r="AJ13" s="17">
-        <v>1.903</v>
+        <v>0.69</v>
       </c>
       <c r="AK13" s="16">
-        <v>-1.49</v>
+        <v>-0.45500000000000002</v>
       </c>
       <c r="AL13" s="16">
-        <v>39.368000000000002</v>
+        <v>12.882</v>
       </c>
       <c r="AM13" s="15">
-        <v>22.577000000000002</v>
+        <v>8.35</v>
       </c>
       <c r="AN13" s="17">
-        <v>7.0860000000000003</v>
+        <v>1.7509999999999999</v>
       </c>
       <c r="AO13" s="16">
-        <v>-3.036</v>
+        <v>-0.77600000000000002</v>
       </c>
       <c r="AP13" s="16">
-        <v>50.679000000000002</v>
+        <v>19.751000000000001</v>
       </c>
       <c r="AQ13" s="15">
-        <v>-23.734000000000002</v>
+        <v>-6.0259999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" s="27">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="26">
         <v>0</v>
       </c>
       <c r="C14" s="23">
-        <v>5</v>
-      </c>
-      <c r="D14" s="24">
+        <v>5.7</v>
+      </c>
+      <c r="D14" s="29">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E14" s="30">
+        <v>9.1</v>
+      </c>
+      <c r="F14" s="24">
+        <v>6.5</v>
+      </c>
+      <c r="G14" s="30">
+        <v>6.9</v>
+      </c>
+      <c r="H14" s="24">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I14" s="23">
+        <v>5.2</v>
+      </c>
+      <c r="J14" s="29">
+        <v>6.3</v>
+      </c>
+      <c r="K14" s="23">
         <v>6</v>
       </c>
-      <c r="E14" s="25">
-        <v>4.5</v>
-      </c>
-      <c r="F14" s="24">
-        <v>8</v>
-      </c>
-      <c r="G14" s="25">
-        <v>7</v>
-      </c>
-      <c r="H14" s="24">
-        <v>6</v>
-      </c>
-      <c r="I14" s="23">
-        <v>3</v>
-      </c>
-      <c r="J14" s="24">
-        <v>3</v>
-      </c>
-      <c r="K14" s="23">
-        <v>9</v>
-      </c>
       <c r="L14" s="23">
-        <v>8</v>
+        <v>6.4</v>
       </c>
       <c r="M14" s="23">
-        <v>3</v>
-      </c>
-      <c r="N14" s="22">
-        <v>2</v>
+        <v>4.8</v>
+      </c>
+      <c r="N14" s="28">
+        <v>5.6</v>
       </c>
       <c r="O14" s="17">
-        <v>824.65</v>
+        <v>2298.15</v>
       </c>
       <c r="P14" s="16">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="Q14" s="15">
-        <v>0.20499999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="R14" s="21">
-        <v>43.367333333333335</v>
+        <v>34.764666666666663</v>
       </c>
       <c r="S14" s="20">
-        <v>70.941999999999993</v>
+        <v>77.349666666666664</v>
       </c>
       <c r="T14" s="19">
-        <v>368.10666666666663</v>
+        <v>415.67</v>
       </c>
       <c r="U14" s="21">
-        <v>43.367333333333335</v>
+        <v>34.764666666666663</v>
       </c>
       <c r="V14" s="20">
-        <v>70.941999999999993</v>
+        <v>77.349666666666664</v>
       </c>
       <c r="W14" s="19">
-        <v>368.10666666666663</v>
+        <v>415.67</v>
       </c>
       <c r="X14" s="18">
-        <v>35.155999999999999</v>
+        <v>27.05</v>
       </c>
       <c r="Y14" s="16">
-        <v>1.5589999999999999</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="Z14" s="15">
-        <v>0.64400000000000002</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="AA14" s="17">
-        <v>1384.55</v>
+        <v>676.67</v>
       </c>
       <c r="AB14" s="16">
-        <v>349.625</v>
+        <v>186.215</v>
       </c>
       <c r="AC14" s="16">
-        <v>0.253</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="AD14" s="16">
-        <v>0.85399999999999998</v>
+        <v>1.28</v>
       </c>
       <c r="AE14" s="16">
-        <v>10.826000000000001</v>
+        <v>7.6</v>
       </c>
       <c r="AF14" s="16">
-        <v>50.44</v>
+        <v>33.344999999999999</v>
       </c>
       <c r="AG14" s="18">
-        <v>34.247</v>
+        <v>43.427999999999997</v>
       </c>
       <c r="AH14" s="17">
-        <v>20.6</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="15">
-        <v>38.4</v>
+        <v>43.65</v>
       </c>
       <c r="AJ14" s="17">
-        <v>2.4769999999999999</v>
+        <v>1.903</v>
       </c>
       <c r="AK14" s="16">
-        <v>-1.9670000000000001</v>
+        <v>-1.49</v>
       </c>
       <c r="AL14" s="16">
-        <v>52.082000000000001</v>
+        <v>39.368000000000002</v>
       </c>
       <c r="AM14" s="15">
-        <v>30.425000000000001</v>
+        <v>22.577000000000002</v>
       </c>
       <c r="AN14" s="17">
-        <v>10.882</v>
+        <v>7.0860000000000003</v>
       </c>
       <c r="AO14" s="16">
-        <v>-4.3440000000000003</v>
+        <v>-3.036</v>
       </c>
       <c r="AP14" s="16">
-        <v>75.668999999999997</v>
+        <v>50.679000000000002</v>
       </c>
       <c r="AQ14" s="15">
-        <v>-33.256999999999998</v>
+        <v>-23.734000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
+        <v>111</v>
+      </c>
+      <c r="B15" s="26">
+        <v>0</v>
+      </c>
+      <c r="C15" s="23">
+        <v>5</v>
+      </c>
+      <c r="D15" s="24">
+        <v>6</v>
+      </c>
+      <c r="E15" s="25">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="24">
+        <v>8</v>
+      </c>
+      <c r="G15" s="25">
+        <v>7</v>
+      </c>
+      <c r="H15" s="24">
+        <v>6</v>
+      </c>
+      <c r="I15" s="23">
+        <v>3</v>
+      </c>
+      <c r="J15" s="24">
+        <v>3</v>
+      </c>
+      <c r="K15" s="23">
+        <v>9</v>
+      </c>
+      <c r="L15" s="23">
+        <v>8</v>
+      </c>
+      <c r="M15" s="23">
+        <v>3</v>
+      </c>
+      <c r="N15" s="22">
+        <v>2</v>
+      </c>
+      <c r="O15" s="17">
+        <v>824.65</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="R15" s="21">
+        <v>43.367333333333335</v>
+      </c>
+      <c r="S15" s="20">
+        <v>70.941999999999993</v>
+      </c>
+      <c r="T15" s="19">
+        <v>368.10666666666663</v>
+      </c>
+      <c r="U15" s="21">
+        <v>43.367333333333335</v>
+      </c>
+      <c r="V15" s="20">
+        <v>70.941999999999993</v>
+      </c>
+      <c r="W15" s="19">
+        <v>368.10666666666663</v>
+      </c>
+      <c r="X15" s="18">
+        <v>35.155999999999999</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AA15" s="17">
+        <v>1384.55</v>
+      </c>
+      <c r="AB15" s="16">
+        <v>349.625</v>
+      </c>
+      <c r="AC15" s="16">
+        <v>0.253</v>
+      </c>
+      <c r="AD15" s="16">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="AE15" s="16">
+        <v>10.826000000000001</v>
+      </c>
+      <c r="AF15" s="16">
+        <v>50.44</v>
+      </c>
+      <c r="AG15" s="18">
+        <v>34.247</v>
+      </c>
+      <c r="AH15" s="17">
+        <v>20.6</v>
+      </c>
+      <c r="AI15" s="15">
+        <v>38.4</v>
+      </c>
+      <c r="AJ15" s="17">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="AK15" s="16">
+        <v>-1.9670000000000001</v>
+      </c>
+      <c r="AL15" s="16">
+        <v>52.082000000000001</v>
+      </c>
+      <c r="AM15" s="15">
+        <v>30.425000000000001</v>
+      </c>
+      <c r="AN15" s="17">
+        <v>10.882</v>
+      </c>
+      <c r="AO15" s="16">
+        <v>-4.3440000000000003</v>
+      </c>
+      <c r="AP15" s="16">
+        <v>75.668999999999997</v>
+      </c>
+      <c r="AQ15" s="15">
+        <v>-33.256999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A16" s="27">
         <v>112</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B16" s="26">
         <v>0.3</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C16" s="23">
         <v>5.6</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D16" s="24">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E16" s="25">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F16" s="24">
         <v>5.2</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G16" s="25">
         <v>4.5</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H16" s="24">
         <v>3.4</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I16" s="23">
         <v>6</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J16" s="24">
         <v>6.1</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K16" s="23">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L16" s="23">
         <v>5.4</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M16" s="23">
         <v>5.7</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N16" s="22">
         <v>5.5</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O16" s="17">
         <v>1219.3499999999999</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P16" s="16">
         <v>0.217</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q16" s="15">
         <v>0.217</v>
       </c>
-      <c r="R15" s="21">
+      <c r="R16" s="21">
         <v>53.756333333333338</v>
       </c>
-      <c r="S15" s="20">
+      <c r="S16" s="20">
         <v>61.565666666666665</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T16" s="19">
         <v>311.50666666666672</v>
       </c>
-      <c r="U15" s="21">
+      <c r="U16" s="21">
         <v>53.756333333333338</v>
       </c>
-      <c r="V15" s="20">
+      <c r="V16" s="20">
         <v>61.565666666666665</v>
       </c>
-      <c r="W15" s="19">
+      <c r="W16" s="19">
         <v>311.50666666666672</v>
       </c>
-      <c r="X15" s="18">
+      <c r="X16" s="18">
         <v>15.22</v>
       </c>
-      <c r="Y15" s="16">
+      <c r="Y16" s="16">
         <v>8.0399999999999991</v>
       </c>
-      <c r="Z15" s="15">
+      <c r="Z16" s="15">
         <v>0.44600000000000001</v>
       </c>
-      <c r="AA15" s="17">
+      <c r="AA16" s="17">
         <v>976.5</v>
       </c>
-      <c r="AB15" s="16">
+      <c r="AB16" s="16">
         <v>436.96499999999997</v>
       </c>
-      <c r="AC15" s="16">
+      <c r="AC16" s="16">
         <v>0.44800000000000001</v>
       </c>
-      <c r="AD15" s="16">
+      <c r="AD16" s="16">
         <v>0.95099999999999996</v>
       </c>
-      <c r="AE15" s="16">
+      <c r="AE16" s="16">
         <v>8.89</v>
       </c>
-      <c r="AF15" s="16">
+      <c r="AF16" s="16">
         <v>63.16</v>
       </c>
-      <c r="AG15" s="18">
+      <c r="AG16" s="18">
         <v>42.54</v>
       </c>
-      <c r="AH15" s="17">
+      <c r="AH16" s="17">
         <v>12.4</v>
       </c>
-      <c r="AI15" s="15">
+      <c r="AI16" s="15">
         <v>22.9</v>
       </c>
-      <c r="AJ15" s="17">
+      <c r="AJ16" s="17">
         <v>4.4530000000000003</v>
       </c>
-      <c r="AK15" s="16">
+      <c r="AK16" s="16">
         <v>-3.36</v>
       </c>
-      <c r="AL15" s="16">
+      <c r="AL16" s="16">
         <v>89.652000000000001</v>
       </c>
-      <c r="AM15" s="15">
+      <c r="AM16" s="15">
         <v>46.76</v>
       </c>
-      <c r="AN15" s="17">
+      <c r="AN16" s="17">
         <v>16.68</v>
       </c>
-      <c r="AO15" s="16">
+      <c r="AO16" s="16">
         <v>-5.8289999999999997</v>
       </c>
-      <c r="AP15" s="16">
+      <c r="AP16" s="16">
         <v>118.86199999999999</v>
       </c>
-      <c r="AQ15" s="15">
+      <c r="AQ16" s="15">
         <v>-42.265000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+    <row r="17" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
         <v>113</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B17" s="13">
         <v>0</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C17" s="10">
         <v>2.4</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D17" s="11">
         <v>4.8</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E17" s="12">
         <v>5.3</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F17" s="11">
         <v>4.7</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G17" s="12">
         <v>5.3</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H17" s="11">
         <v>8.5</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I17" s="10">
         <v>4.5</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J17" s="11">
         <v>3.3</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K17" s="10">
         <v>9.1999999999999993</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L17" s="10">
         <v>6.2</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M17" s="10">
         <v>3.2</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N17" s="9">
         <v>1.6</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O17" s="4">
         <v>3415.95</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P17" s="3">
         <v>0.76100000000000001</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q17" s="2">
         <v>0.76100000000000001</v>
       </c>
-      <c r="R16" s="8">
+      <c r="R17" s="8">
         <v>64.486333333333334</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S17" s="7">
         <v>58.567666666666668</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T17" s="6">
         <v>244.14333333333335</v>
       </c>
-      <c r="U16" s="8">
+      <c r="U17" s="8">
         <v>64.486333333333334</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V17" s="7">
         <v>58.567666666666668</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W17" s="6">
         <v>244.14333333333335</v>
       </c>
-      <c r="X16" s="5">
+      <c r="X17" s="5">
         <v>89.974000000000004</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y17" s="3">
         <v>16.675999999999998</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="Z17" s="2">
         <v>0.53600000000000003</v>
       </c>
-      <c r="AA16" s="4">
+      <c r="AA17" s="4">
         <v>4151.5</v>
       </c>
-      <c r="AB16" s="3">
+      <c r="AB17" s="3">
         <v>1106.9000000000001</v>
       </c>
-      <c r="AC16" s="3">
+      <c r="AC17" s="3">
         <v>0.26700000000000002</v>
       </c>
-      <c r="AD16" s="3">
+      <c r="AD17" s="3">
         <v>0.81399999999999995</v>
       </c>
-      <c r="AE16" s="3">
+      <c r="AE17" s="3">
         <v>31.515000000000001</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="AF17" s="3">
         <v>112.65</v>
       </c>
-      <c r="AG16" s="5">
+      <c r="AG17" s="5">
         <v>8.9550000000000001</v>
       </c>
-      <c r="AH16" s="4">
+      <c r="AH17" s="4">
         <v>49.1</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AI17" s="2">
         <v>70.150000000000006</v>
       </c>
-      <c r="AJ16" s="4">
+      <c r="AJ17" s="4">
         <v>7.3630000000000004</v>
       </c>
-      <c r="AK16" s="3">
+      <c r="AK17" s="3">
         <v>-6.1369999999999996</v>
       </c>
-      <c r="AL16" s="3">
+      <c r="AL17" s="3">
         <v>153.86000000000001</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AM17" s="2">
         <v>100.20699999999999</v>
       </c>
-      <c r="AN16" s="4">
+      <c r="AN17" s="4">
         <v>32.517000000000003</v>
       </c>
-      <c r="AO16" s="3">
+      <c r="AO17" s="3">
         <v>-11.042999999999999</v>
       </c>
-      <c r="AP16" s="3">
+      <c r="AP17" s="3">
         <v>235.32599999999999</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="AQ17" s="2">
         <v>-79.501000000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="AA2:AI2"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="O1:AI1"/>
-    <mergeCell ref="AJ1:AQ1"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="O2:Z2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="AA3:AI3"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="O2:AI2"/>
+    <mergeCell ref="AJ2:AQ2"/>
+    <mergeCell ref="AJ3:AM3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="O3:Z3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add upload data and some button (but not fonctionnal)
</commit_message>
<xml_diff>
--- a/Doc/Emulsion_Recap.xlsx
+++ b/Doc/Emulsion_Recap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Bureau\Moi\Efrei\Imbartabac\Programme\Assistanat_Project\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12680A-AAD5-4341-B1C8-1A220692DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911FA609-A8D3-4988-B6A0-1ACFF32A09FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
   </bookViews>
   <sheets>
     <sheet name="Récapitulatif" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Aminus</t>
   </si>
@@ -177,9 +177,6 @@
     <t>G1</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -283,6 +280,12 @@
   </si>
   <si>
     <t>ANALYSE SENSORIELLE</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
   </si>
 </sst>
 </file>
@@ -1629,8 +1632,8 @@
   </sheetPr>
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="AG5" workbookViewId="0">
+      <selection activeCell="AN21" sqref="AN21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,7 +1654,7 @@
     <row r="2" spans="1:43" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="75"/>
       <c r="B2" s="82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="83"/>
@@ -1666,7 +1669,7 @@
       <c r="M2" s="83"/>
       <c r="N2" s="84"/>
       <c r="O2" s="85" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P2" s="86"/>
       <c r="Q2" s="86"/>
@@ -1689,7 +1692,7 @@
       <c r="AH2" s="86"/>
       <c r="AI2" s="87"/>
       <c r="AJ2" s="88" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AK2" s="89"/>
       <c r="AL2" s="89"/>
@@ -1702,30 +1705,30 @@
     <row r="3" spans="1:43" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="74"/>
       <c r="B3" s="76" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="77"/>
       <c r="D3" s="77"/>
       <c r="E3" s="76" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="78"/>
       <c r="G3" s="77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="77"/>
       <c r="I3" s="76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="78"/>
       <c r="K3" s="76" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" s="77"/>
       <c r="M3" s="77"/>
       <c r="N3" s="78"/>
       <c r="O3" s="79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="80"/>
       <c r="Q3" s="80"/>
@@ -1739,7 +1742,7 @@
       <c r="Y3" s="80"/>
       <c r="Z3" s="81"/>
       <c r="AA3" s="79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB3" s="80"/>
       <c r="AC3" s="80"/>
@@ -1750,13 +1753,13 @@
       <c r="AH3" s="80"/>
       <c r="AI3" s="81"/>
       <c r="AJ3" s="91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AK3" s="92"/>
       <c r="AL3" s="92"/>
       <c r="AM3" s="93"/>
       <c r="AN3" s="91" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO3" s="92"/>
       <c r="AP3" s="92"/>
@@ -1765,79 +1768,79 @@
     <row r="4" spans="1:43" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="73"/>
       <c r="B4" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" s="69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" s="70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="69" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N4" s="68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="V4" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y4" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="66" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="U4" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="V4" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="X4" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y4" s="61" t="s">
-        <v>18</v>
-      </c>
       <c r="Z4" s="60" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="AA4" s="59" t="s">
         <v>16</v>
@@ -2614,7 +2617,7 @@
         <v>78.012</v>
       </c>
       <c r="W10" s="19">
-        <v>417.57333333333332</v>
+        <v>417.57333333333298</v>
       </c>
       <c r="X10" s="18">
         <v>28.992000000000001</v>

</xml_diff>

<commit_message>
add optionnal only instru or senso
</commit_message>
<xml_diff>
--- a/Doc/Emulsion_Recap.xlsx
+++ b/Doc/Emulsion_Recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Bureau\Moi\Efrei\Imbartabac\Programme\Assistanat_Project\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911FA609-A8D3-4988-B6A0-1ACFF32A09FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7AA2A-8B21-436E-955B-883D46697116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A344C62-2E7F-4919-9530-7E0837607192}"/>
   </bookViews>
   <sheets>
     <sheet name="Récapitulatif" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Aminus</t>
   </si>
@@ -286,6 +286,45 @@
   </si>
   <si>
     <t>n2</t>
+  </si>
+  <si>
+    <t>produit 101</t>
+  </si>
+  <si>
+    <t>produit 102</t>
+  </si>
+  <si>
+    <t>produit 103</t>
+  </si>
+  <si>
+    <t>produit 104</t>
+  </si>
+  <si>
+    <t>produit 105</t>
+  </si>
+  <si>
+    <t>produit 106</t>
+  </si>
+  <si>
+    <t>produit 107</t>
+  </si>
+  <si>
+    <t>produit 108</t>
+  </si>
+  <si>
+    <t>produit 109</t>
+  </si>
+  <si>
+    <t>produit 110</t>
+  </si>
+  <si>
+    <t>produit 111</t>
+  </si>
+  <si>
+    <t>produit 112</t>
+  </si>
+  <si>
+    <t>produit 113</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG5" workbookViewId="0">
-      <selection activeCell="AN21" sqref="AN21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1895,8 +1934,8 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A5" s="54">
-        <v>101</v>
+      <c r="A5" s="54" t="s">
+        <v>54</v>
       </c>
       <c r="B5" s="53">
         <v>0</v>
@@ -2026,8 +2065,8 @@
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
-        <v>102</v>
+      <c r="A6" s="27" t="s">
+        <v>55</v>
       </c>
       <c r="B6" s="26">
         <v>0</v>
@@ -2157,8 +2196,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
-        <v>103</v>
+      <c r="A7" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
@@ -2288,8 +2327,8 @@
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>104</v>
+      <c r="A8" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="B8" s="26">
         <v>0</v>
@@ -2419,8 +2458,8 @@
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
-        <v>105</v>
+      <c r="A9" s="27" t="s">
+        <v>58</v>
       </c>
       <c r="B9" s="26">
         <v>0</v>
@@ -2550,8 +2589,8 @@
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
-        <v>106</v>
+      <c r="A10" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B10" s="26">
         <v>0</v>
@@ -2681,8 +2720,8 @@
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
-        <v>107</v>
+      <c r="A11" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="B11" s="26">
         <v>0.2</v>
@@ -2812,8 +2851,8 @@
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
-        <v>108</v>
+      <c r="A12" s="27" t="s">
+        <v>61</v>
       </c>
       <c r="B12" s="26">
         <v>0</v>
@@ -2943,8 +2982,8 @@
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
-        <v>109</v>
+      <c r="A13" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="B13" s="26">
         <v>5</v>
@@ -3074,8 +3113,8 @@
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
-        <v>110</v>
+      <c r="A14" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="B14" s="26">
         <v>0</v>
@@ -3205,8 +3244,8 @@
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A15" s="27">
-        <v>111</v>
+      <c r="A15" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="B15" s="26">
         <v>0</v>
@@ -3336,8 +3375,8 @@
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
-        <v>112</v>
+      <c r="A16" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="B16" s="26">
         <v>0.3</v>
@@ -3467,8 +3506,8 @@
       </c>
     </row>
     <row r="17" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
-        <v>113</v>
+      <c r="A17" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>

</xml_diff>